<commit_message>
crud and script for alterated the db
</commit_message>
<xml_diff>
--- a/data/xlsx/03 datos insertar.xlsx
+++ b/data/xlsx/03 datos insertar.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\P Y T H O N\4 - Opalo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hinojsa/Desktop/jupiter/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FE6A90-5837-7C4C-B040-B7B595E21338}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680"/>
+    <workbookView xWindow="16400" yWindow="500" windowWidth="20460" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="historico_tasas_gen" sheetId="7" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="82">
   <si>
     <t>fecha</t>
   </si>
@@ -268,12 +269,18 @@
   </si>
   <si>
     <t>true</t>
+  </si>
+  <si>
+    <t>pk_control</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -332,7 +339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -340,10 +347,12 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -620,27 +629,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="3"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" style="3"/>
+    <col min="2" max="2" width="10.83203125" style="8"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -661,10 +671,13 @@
       <c r="H1" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
-      <c r="B2" s="1">
+      <c r="B2" s="8">
         <v>44298</v>
       </c>
       <c r="C2" s="6">
@@ -679,10 +692,13 @@
       <c r="F2" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
-      <c r="B3" s="1">
+      <c r="B3" s="8">
         <v>44298</v>
       </c>
       <c r="C3" s="6">
@@ -697,10 +713,13 @@
       <c r="F3" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
-      <c r="B4" s="1">
+      <c r="B4" s="8">
         <v>44298</v>
       </c>
       <c r="C4" s="6">
@@ -715,10 +734,13 @@
       <c r="F4" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
-      <c r="B5" s="1">
+      <c r="B5" s="8">
         <v>44298</v>
       </c>
       <c r="C5" s="6">
@@ -733,10 +755,13 @@
       <c r="F5" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
-      <c r="B6" s="1">
+      <c r="B6" s="8">
         <v>44298</v>
       </c>
       <c r="C6" s="6">
@@ -751,10 +776,13 @@
       <c r="F6" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
-      <c r="B7" s="1">
+      <c r="B7" s="8">
         <v>44298</v>
       </c>
       <c r="C7" s="6">
@@ -769,10 +797,13 @@
       <c r="F7" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
-      <c r="B8" s="1">
+      <c r="B8" s="8">
         <v>44298</v>
       </c>
       <c r="C8" s="6">
@@ -787,10 +818,13 @@
       <c r="F8" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="1">
+      <c r="B9" s="8">
         <v>44298</v>
       </c>
       <c r="C9" s="6">
@@ -805,10 +839,13 @@
       <c r="F9" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
-      <c r="B10" s="1">
+      <c r="B10" s="8">
         <v>44298</v>
       </c>
       <c r="C10" s="6">
@@ -823,10 +860,13 @@
       <c r="F10" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
-      <c r="B11" s="1">
+      <c r="B11" s="8">
         <v>44298</v>
       </c>
       <c r="C11" s="6">
@@ -844,10 +884,13 @@
       <c r="G11" s="6">
         <v>102</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
-      <c r="B12" s="1">
+      <c r="B12" s="8">
         <v>44298</v>
       </c>
       <c r="C12" s="6">
@@ -865,10 +908,13 @@
       <c r="G12" s="6">
         <v>104</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
-      <c r="B13" s="1">
+      <c r="B13" s="8">
         <v>44298</v>
       </c>
       <c r="C13" s="6">
@@ -886,10 +932,13 @@
       <c r="G13" s="6">
         <v>105</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
-      <c r="B14" s="1">
+      <c r="B14" s="8">
         <v>44298</v>
       </c>
       <c r="C14" s="6">
@@ -907,10 +956,13 @@
       <c r="G14" s="6">
         <v>106</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
-      <c r="B15" s="1">
+      <c r="B15" s="8">
         <v>44298</v>
       </c>
       <c r="C15" s="6">
@@ -928,10 +980,13 @@
       <c r="G15" s="6">
         <v>107</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
-      <c r="B16" s="1">
+      <c r="B16" s="8">
         <v>44298</v>
       </c>
       <c r="C16" s="6">
@@ -949,10 +1004,13 @@
       <c r="G16" s="6">
         <v>108</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
-      <c r="B17" s="1">
+      <c r="B17" s="8">
         <v>44298</v>
       </c>
       <c r="C17" s="6">
@@ -970,10 +1028,13 @@
       <c r="G17" s="6">
         <v>109</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
-      <c r="B18" s="1">
+      <c r="B18" s="8">
         <v>44298</v>
       </c>
       <c r="C18" s="6">
@@ -991,10 +1052,13 @@
       <c r="G18" s="6">
         <v>110</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
-      <c r="B19" s="1">
+      <c r="B19" s="8">
         <v>44298</v>
       </c>
       <c r="C19" s="6">
@@ -1012,10 +1076,13 @@
       <c r="G19" s="6">
         <v>103</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
-      <c r="B20" s="1">
+      <c r="B20" s="8">
         <v>44298</v>
       </c>
       <c r="C20" s="6">
@@ -1033,10 +1100,13 @@
       <c r="G20" s="6">
         <v>101</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
-      <c r="B21" s="1">
+      <c r="B21" s="8">
         <v>44298</v>
       </c>
       <c r="C21" s="6">
@@ -1050,6 +1120,9 @@
       </c>
       <c r="F21" s="6" t="s">
         <v>80</v>
+      </c>
+      <c r="I21">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1059,16 +1132,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BI3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:61" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:61" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1253,7 +1326,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44298</v>
       </c>
@@ -1436,7 +1509,7 @@
       </c>
       <c r="BI2" s="6"/>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
     </row>
   </sheetData>

</xml_diff>